<commit_message>
Fix map farm locations so that everything is in or close to King county
</commit_message>
<xml_diff>
--- a/Data/farm_coords.xlsx
+++ b/Data/farm_coords.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\starr\Google Drive\Main Projects\Harvest Against Hunger Summer '21\harvest-against-hunger\Datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\starr\Google Drive\Career Projects\Projects\Harvest Against Hunger Summer '21\harvest-against-hunger\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86DDD7A-523E-4701-BB58-E6FC49A95522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F95171-BD59-4D86-B4E1-60447201FA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -235,9 +235,6 @@
     <t>47.3950706,-122.2297455</t>
   </si>
   <si>
-    <t>47.8807116,-122.0508067</t>
-  </si>
-  <si>
     <t>47.3266708,-122.232777</t>
   </si>
   <si>
@@ -250,9 +247,6 @@
     <t>47.5697033,-122.3504832</t>
   </si>
   <si>
-    <t>47.9273634,-122.110984</t>
-  </si>
-  <si>
     <t>47.4794336,-122.4706857</t>
   </si>
   <si>
@@ -268,12 +262,6 @@
     <t>47.6063486,-121.9331677</t>
   </si>
   <si>
-    <t>47.837332,-121.9423236</t>
-  </si>
-  <si>
-    <t>47.8097676,-122.1437116</t>
-  </si>
-  <si>
     <t>47.5273011,-121.8707362</t>
   </si>
   <si>
@@ -286,12 +274,6 @@
     <t>45.6133416,-122.4376827</t>
   </si>
   <si>
-    <t>47.4209319,-122.7308538</t>
-  </si>
-  <si>
-    <t>47.842929,-122.086635</t>
-  </si>
-  <si>
     <t>47.4323906,-122.4666727</t>
   </si>
   <si>
@@ -304,18 +286,9 @@
     <t>New Roots Farm Program</t>
   </si>
   <si>
-    <t>45.4339212,-122.4022518</t>
-  </si>
-  <si>
-    <t>44.346267,-117.1387678</t>
-  </si>
-  <si>
     <t>47.4252238,-122.4714232</t>
   </si>
   <si>
-    <t>47.9273501,-122.0811616</t>
-  </si>
-  <si>
     <t>47.6658059,-122.0312807</t>
   </si>
   <si>
@@ -340,9 +313,6 @@
     <t>47.7506474,-122.1783049</t>
   </si>
   <si>
-    <t>47.8414202,-122.0815436</t>
-  </si>
-  <si>
     <t>47.2216756,-122.0539346</t>
   </si>
   <si>
@@ -394,10 +364,40 @@
     <t>47.4565606,-122.4511177</t>
   </si>
   <si>
-    <t>47.8642506,-121.9477157</t>
-  </si>
-  <si>
     <t>47.4233042,-122.4477158</t>
+  </si>
+  <si>
+    <t>47.6777367,-122.0058828</t>
+  </si>
+  <si>
+    <t>47.3239497,-122.2772907</t>
+  </si>
+  <si>
+    <t>47.6349728,-122.0819622</t>
+  </si>
+  <si>
+    <t>47.6757423,-122.2394706</t>
+  </si>
+  <si>
+    <t>47.8877264,-121.7938542</t>
+  </si>
+  <si>
+    <t>47.8634311,-121.9435757</t>
+  </si>
+  <si>
+    <t>47.8782821,-122.0526352</t>
+  </si>
+  <si>
+    <t>47.836134,-122.0852195</t>
+  </si>
+  <si>
+    <t>47.8062607,-122.122593</t>
+  </si>
+  <si>
+    <t>47.7605015,-122.3874161</t>
+  </si>
+  <si>
+    <t>47.5555656,-122.3209544</t>
   </si>
 </sst>
 </file>
@@ -786,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,15 +874,15 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -890,7 +890,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -898,7 +898,7 @@
         <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -906,7 +906,7 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -914,7 +914,7 @@
         <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -922,7 +922,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -930,7 +930,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -938,7 +938,7 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -946,7 +946,7 @@
         <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -954,7 +954,7 @@
         <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -962,7 +962,7 @@
         <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -970,7 +970,7 @@
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -978,7 +978,7 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -986,7 +986,7 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -994,7 +994,7 @@
         <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1002,7 +1002,7 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1010,7 +1010,7 @@
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1018,7 +1018,7 @@
         <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1026,7 +1026,7 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1034,7 +1034,7 @@
         <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1042,7 +1042,7 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1050,7 +1050,7 @@
         <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1058,15 +1058,15 @@
         <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B34" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1074,7 +1074,7 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1082,7 +1082,7 @@
         <v>61</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1090,7 +1090,7 @@
         <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1098,7 +1098,7 @@
         <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1106,7 +1106,7 @@
         <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1114,7 +1114,7 @@
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1122,7 +1122,7 @@
         <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1130,7 +1130,7 @@
         <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1138,7 +1138,7 @@
         <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1146,7 +1146,7 @@
         <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1154,7 +1154,7 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1162,7 +1162,7 @@
         <v>60</v>
       </c>
       <c r="B46" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1170,7 +1170,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1178,7 +1178,7 @@
         <v>25</v>
       </c>
       <c r="B48" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1186,7 +1186,7 @@
         <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1194,7 +1194,7 @@
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1202,7 +1202,7 @@
         <v>39</v>
       </c>
       <c r="B51" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1210,7 +1210,7 @@
         <v>31</v>
       </c>
       <c r="B52" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1218,7 +1218,7 @@
         <v>29</v>
       </c>
       <c r="B53" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1226,7 +1226,7 @@
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1234,7 +1234,7 @@
         <v>13</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1242,7 +1242,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1250,7 +1250,7 @@
         <v>22</v>
       </c>
       <c r="B57" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1258,7 +1258,7 @@
         <v>41</v>
       </c>
       <c r="B58" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1266,7 +1266,7 @@
         <v>28</v>
       </c>
       <c r="B59" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1274,7 +1274,7 @@
         <v>32</v>
       </c>
       <c r="B60" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1282,7 +1282,7 @@
         <v>17</v>
       </c>
       <c r="B61" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1290,7 +1290,7 @@
         <v>46</v>
       </c>
       <c r="B62" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1298,7 +1298,7 @@
         <v>34</v>
       </c>
       <c r="B63" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1306,7 +1306,7 @@
         <v>5</v>
       </c>
       <c r="B64" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>